<commit_message>
xuất file quy hoach chi tiet
</commit_message>
<xml_diff>
--- a/WebGISQuangNam/WebGISQuangNam/Resources/MauPhieu/MauPhieuThongTin_GIS.xlsx
+++ b/WebGISQuangNam/WebGISQuangNam/Resources/MauPhieu/MauPhieuThongTin_GIS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>www.gisquyhoach.quangnam.vn</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Khoảng lùi chính:</t>
+  </si>
+  <si>
+    <t>Ghi chú: các thuộc tính kí hiệu, địa chỉ, điện thoại, email: chưa rõ thông tin.</t>
   </si>
 </sst>
 </file>
@@ -228,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -246,11 +249,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -264,9 +270,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ25"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14:AB14"/>
+      <selection activeCell="U23" sqref="U23:AB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -798,100 +802,100 @@
       <c r="AD4" s="7"/>
     </row>
     <row r="5" spans="1:36" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
     </row>
     <row r="6" spans="1:36" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16"/>
     </row>
     <row r="7" spans="1:36" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:36" ht="177.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="17"/>
-      <c r="AA8" s="17"/>
-      <c r="AB8" s="18"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="19"/>
     </row>
     <row r="9" spans="1:36" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="8" t="s">
@@ -931,26 +935,26 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="19"/>
-      <c r="Z11" s="19"/>
-      <c r="AA11" s="19"/>
-      <c r="AB11" s="19"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="D12" s="3" t="s">
@@ -960,26 +964,26 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="19"/>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="19"/>
-      <c r="Z12" s="19"/>
-      <c r="AA12" s="19"/>
-      <c r="AB12" s="19"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="15"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="D13" s="3" t="s">
@@ -989,26 +993,26 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19"/>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="19"/>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="19"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="D14" s="3" t="s">
@@ -1020,28 +1024,28 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
       <c r="N14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="O14" s="3"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="19"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
       <c r="U14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="V14" s="3"/>
-      <c r="W14" s="19"/>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="19"/>
-      <c r="AA14" s="19"/>
-      <c r="AB14" s="19"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
     </row>
     <row r="15" spans="1:36" ht="10.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:36" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -1082,12 +1086,12 @@
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12" t="s">
         <v>12</v>
@@ -1096,14 +1100,14 @@
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="14"/>
-      <c r="Y18" s="14"/>
-      <c r="Z18" s="14"/>
-      <c r="AA18" s="14"/>
-      <c r="AB18" s="14"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="13"/>
+      <c r="AB18" s="13"/>
     </row>
     <row r="19" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D19" s="12" t="s">
@@ -1113,12 +1117,12 @@
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
       <c r="O19" s="12"/>
       <c r="P19" s="12" t="s">
         <v>13</v>
@@ -1127,14 +1131,14 @@
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
       <c r="T19" s="12"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="14"/>
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="13"/>
     </row>
     <row r="20" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D20" s="12" t="s">
@@ -1144,12 +1148,12 @@
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12" t="s">
         <v>14</v>
@@ -1158,14 +1162,14 @@
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
       <c r="T20" s="12"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="14"/>
-      <c r="X20" s="14"/>
-      <c r="Y20" s="14"/>
-      <c r="Z20" s="14"/>
-      <c r="AA20" s="14"/>
-      <c r="AB20" s="14"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+      <c r="AA20" s="13"/>
+      <c r="AB20" s="13"/>
     </row>
     <row r="21" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D21" s="12" t="s">
@@ -1175,12 +1179,12 @@
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12" t="s">
         <v>15</v>
@@ -1189,14 +1193,14 @@
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
       <c r="T21" s="12"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="14"/>
-      <c r="Y21" s="14"/>
-      <c r="Z21" s="14"/>
-      <c r="AA21" s="14"/>
-      <c r="AB21" s="14"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="13"/>
     </row>
     <row r="22" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D22" s="12" t="s">
@@ -1206,12 +1210,12 @@
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
       <c r="O22" s="12"/>
       <c r="P22" s="12" t="s">
         <v>16</v>
@@ -1220,14 +1224,14 @@
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
       <c r="T22" s="12"/>
-      <c r="U22" s="14"/>
-      <c r="V22" s="14"/>
-      <c r="W22" s="14"/>
-      <c r="X22" s="14"/>
-      <c r="Y22" s="14"/>
-      <c r="Z22" s="14"/>
-      <c r="AA22" s="14"/>
-      <c r="AB22" s="14"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="13"/>
     </row>
     <row r="23" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D23" s="12" t="s">
@@ -1237,12 +1241,12 @@
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
       <c r="O23" s="12"/>
       <c r="P23" s="12" t="s">
         <v>21</v>
@@ -1251,14 +1255,14 @@
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
       <c r="T23" s="12"/>
-      <c r="U23" s="14"/>
-      <c r="V23" s="14"/>
-      <c r="W23" s="14"/>
-      <c r="X23" s="14"/>
-      <c r="Y23" s="14"/>
-      <c r="Z23" s="14"/>
-      <c r="AA23" s="14"/>
-      <c r="AB23" s="14"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="13"/>
     </row>
     <row r="24" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D24" s="12" t="s">
@@ -1268,26 +1272,26 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="14"/>
-      <c r="Y24" s="14"/>
-      <c r="Z24" s="14"/>
-      <c r="AA24" s="14"/>
-      <c r="AB24" s="14"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="13"/>
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="13"/>
     </row>
     <row r="25" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D25" s="12" t="s">
@@ -1297,12 +1301,12 @@
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
       <c r="O25" s="12"/>
       <c r="P25" s="12" t="s">
         <v>24</v>
@@ -1311,25 +1315,22 @@
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
       <c r="T25" s="12"/>
-      <c r="U25" s="14"/>
-      <c r="V25" s="14"/>
-      <c r="W25" s="14"/>
-      <c r="X25" s="14"/>
-      <c r="Y25" s="14"/>
-      <c r="Z25" s="14"/>
-      <c r="AA25" s="14"/>
-      <c r="AB25" s="14"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="13"/>
+      <c r="Z25" s="13"/>
+      <c r="AA25" s="13"/>
+      <c r="AB25" s="13"/>
+    </row>
+    <row r="30" spans="4:28" x14ac:dyDescent="0.3">
+      <c r="D30" s="20" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="U21:AB21"/>
-    <mergeCell ref="U23:AB23"/>
-    <mergeCell ref="U22:AB22"/>
-    <mergeCell ref="I24:AB24"/>
-    <mergeCell ref="U25:AB25"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I23:N23"/>
-    <mergeCell ref="I25:N25"/>
     <mergeCell ref="A5:AD5"/>
     <mergeCell ref="P14:T14"/>
     <mergeCell ref="I21:N21"/>
@@ -1346,6 +1347,14 @@
     <mergeCell ref="W14:AB14"/>
     <mergeCell ref="U19:AB19"/>
     <mergeCell ref="U20:AB20"/>
+    <mergeCell ref="U21:AB21"/>
+    <mergeCell ref="U23:AB23"/>
+    <mergeCell ref="U22:AB22"/>
+    <mergeCell ref="I24:AB24"/>
+    <mergeCell ref="U25:AB25"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I23:N23"/>
+    <mergeCell ref="I25:N25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>